<commit_message>
Added code for Excel read & write operation
</commit_message>
<xml_diff>
--- a/src/test/resources/transactionalData.xlsx
+++ b/src/test/resources/transactionalData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>Order ID</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>03/11/2025</t>
+  </si>
+  <si>
+    <t>1958442</t>
+  </si>
+  <si>
+    <t>04/16/2025</t>
   </si>
 </sst>
 </file>
@@ -439,7 +445,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
@@ -608,6 +614,17 @@
         <v>17</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>